<commit_message>
fixed tests working implementation for csv files
</commit_message>
<xml_diff>
--- a/tests/test_excelparameterloader.xlsx
+++ b/tests/test_excelparameterloader.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modeling-tools/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/python-table-data-reader/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE8BB9A-220D-C34E-A374-E3DCBCEFD9AF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783BEA3E-53DC-9640-A59C-AC2741A5E245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,18 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="shuffle_col_order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -630,7 +638,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,12 +1133,14 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I20" s="11">
         <v>0.1</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="3">
+        <v>39814</v>
+      </c>
       <c r="K20" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>